<commit_message>
Documentation + User Testing update
</commit_message>
<xml_diff>
--- a/SprintBacklog/Sprint6.xlsx
+++ b/SprintBacklog/Sprint6.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="29">
   <si>
     <t>Sprint Backlog</t>
   </si>
@@ -105,7 +105,22 @@
     <t>Images</t>
   </si>
   <si>
-    <t>Mon 2nd Mar 2015 - Mon 23rd Mar 2014</t>
+    <t>The ability to delete recipes and cookbooks</t>
+  </si>
+  <si>
+    <t>Database design</t>
+  </si>
+  <si>
+    <t>Application code</t>
+  </si>
+  <si>
+    <t>Database code</t>
+  </si>
+  <si>
+    <t>Sync code</t>
+  </si>
+  <si>
+    <t>Mon 2nd Mar 2015 - Mon 16h Mar 2015</t>
   </si>
 </sst>
 </file>
@@ -213,7 +228,14 @@
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="66">
+  <dxfs count="50">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -245,13 +267,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -280,6 +295,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -301,13 +323,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -336,6 +351,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -357,13 +379,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -392,6 +407,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -413,13 +435,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -469,13 +484,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -497,6 +505,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -540,118 +555,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -687,8 +590,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="65"/>
-      <tableStyleElement type="headerRow" dxfId="64"/>
+      <tableStyleElement type="wholeTable" dxfId="49"/>
+      <tableStyleElement type="headerRow" dxfId="48"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -994,10 +897,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V16"/>
+  <dimension ref="A1:V21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U12" sqref="U12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1013,7 +916,7 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="V2" s="4" t="s">
         <v>13</v>
@@ -1130,55 +1033,55 @@
       <c r="A8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="8">
         <v>120</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="3">
+        <v>14</v>
+      </c>
+      <c r="D8" s="8">
         <v>120</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="8">
         <v>110</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="8">
         <v>100</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="8">
+        <v>60</v>
+      </c>
+      <c r="H8" s="8">
+        <v>30</v>
+      </c>
+      <c r="I8" s="8">
+        <v>20</v>
+      </c>
+      <c r="J8" s="8">
+        <v>20</v>
+      </c>
+      <c r="K8" s="8">
+        <v>20</v>
+      </c>
+      <c r="L8" s="8">
+        <v>20</v>
+      </c>
+      <c r="M8" s="8">
         <v>0</v>
       </c>
-      <c r="H8" s="3">
+      <c r="N8" s="8">
         <v>0</v>
       </c>
-      <c r="I8" s="3">
+      <c r="O8" s="8">
         <v>0</v>
       </c>
-      <c r="J8" s="3">
+      <c r="P8" s="8">
         <v>0</v>
       </c>
-      <c r="K8" s="3">
+      <c r="Q8" s="8">
         <v>0</v>
       </c>
-      <c r="L8" s="3">
-        <v>0</v>
-      </c>
-      <c r="M8" s="3">
-        <v>0</v>
-      </c>
-      <c r="N8" s="3">
-        <v>0</v>
-      </c>
-      <c r="O8" s="3">
-        <v>0</v>
-      </c>
-      <c r="P8" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="3">
-        <v>0</v>
-      </c>
-      <c r="R8" s="3">
+      <c r="R8" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1203,274 +1106,587 @@
       <c r="R9" s="3"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
+      <c r="A10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="O11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="P11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="R11" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="A11" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="8">
+        <v>10</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="8">
+        <v>10</v>
+      </c>
+      <c r="E11" s="8">
+        <v>10</v>
+      </c>
+      <c r="F11" s="8">
+        <v>10</v>
+      </c>
+      <c r="G11" s="8">
+        <v>10</v>
+      </c>
+      <c r="H11" s="8">
+        <v>10</v>
+      </c>
+      <c r="I11" s="8">
+        <v>10</v>
+      </c>
+      <c r="J11" s="8">
+        <v>10</v>
+      </c>
+      <c r="K11" s="8">
+        <v>10</v>
+      </c>
+      <c r="L11" s="8">
+        <v>10</v>
+      </c>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>11</v>
+      <c r="A12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="8">
+        <v>40</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
+      <c r="D12" s="8">
+        <v>40</v>
+      </c>
+      <c r="E12" s="8">
+        <v>40</v>
+      </c>
+      <c r="F12" s="8">
+        <v>40</v>
+      </c>
+      <c r="G12" s="8">
+        <v>40</v>
+      </c>
+      <c r="H12" s="8">
+        <v>40</v>
+      </c>
+      <c r="I12" s="8">
+        <v>40</v>
+      </c>
+      <c r="J12" s="8">
+        <v>40</v>
+      </c>
+      <c r="K12" s="8">
+        <v>40</v>
+      </c>
+      <c r="L12" s="8">
+        <v>40</v>
+      </c>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>11</v>
+      <c r="A13" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="8">
+        <v>30</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
+      <c r="D13" s="8">
+        <v>30</v>
+      </c>
+      <c r="E13" s="8">
+        <v>30</v>
+      </c>
+      <c r="F13" s="8">
+        <v>30</v>
+      </c>
+      <c r="G13" s="8">
+        <v>30</v>
+      </c>
+      <c r="H13" s="8">
+        <v>30</v>
+      </c>
+      <c r="I13" s="8">
+        <v>30</v>
+      </c>
+      <c r="J13" s="8">
+        <v>30</v>
+      </c>
+      <c r="K13" s="8">
+        <v>30</v>
+      </c>
+      <c r="L13" s="8">
+        <v>30</v>
+      </c>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" t="s">
-        <v>11</v>
+        <v>27</v>
+      </c>
+      <c r="B14" s="8">
+        <v>60</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>13</v>
       </c>
+      <c r="D14" s="8">
+        <v>60</v>
+      </c>
+      <c r="E14" s="8">
+        <v>60</v>
+      </c>
+      <c r="F14" s="8">
+        <v>60</v>
+      </c>
+      <c r="G14" s="8">
+        <v>60</v>
+      </c>
+      <c r="H14" s="8">
+        <v>60</v>
+      </c>
+      <c r="I14" s="8">
+        <v>60</v>
+      </c>
+      <c r="J14" s="8">
+        <v>60</v>
+      </c>
+      <c r="K14" s="8">
+        <v>60</v>
+      </c>
+      <c r="L14" s="8">
+        <v>60</v>
+      </c>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="8"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="P17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="R17" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B15">
-        <f>SUM(B4:B11)</f>
-        <v>120</v>
-      </c>
-      <c r="D15">
-        <f>SUM(D4:D14)</f>
-        <v>120</v>
-      </c>
-      <c r="E15">
-        <f>SUM(E4:E11)</f>
-        <v>110</v>
-      </c>
-      <c r="F15">
-        <f>SUM(F4:F11)</f>
-        <v>100</v>
-      </c>
-      <c r="G15">
-        <f>SUM(G4:G11)</f>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21">
+        <f>SUM(B4:B17)</f>
+        <v>260</v>
+      </c>
+      <c r="D21">
+        <f>SUM(D4:D20)</f>
+        <v>260</v>
+      </c>
+      <c r="E21">
+        <f t="shared" ref="E21:J21" si="0">SUM(E4:E17)</f>
+        <v>250</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>170</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+      <c r="K21">
+        <f t="shared" ref="K21:Q21" si="1">SUM(K4:K20)</f>
+        <v>160</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H15">
-        <f>SUM(H4:H11)</f>
+      <c r="N21">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I15">
-        <f>SUM(I4:I11)</f>
+      <c r="O21">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J15">
-        <f>SUM(J4:J11)</f>
+      <c r="P21">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K15">
-        <f>SUM(K4:K14)</f>
+      <c r="Q21">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L15">
-        <f>SUM(L4:L14)</f>
+      <c r="R21">
+        <f>SUM(R1:R17)</f>
         <v>0</v>
       </c>
-      <c r="M15">
-        <f>SUM(M4:M14)</f>
-        <v>0</v>
-      </c>
-      <c r="N15">
-        <f>SUM(N4:N14)</f>
-        <v>0</v>
-      </c>
-      <c r="O15">
-        <f>SUM(O4:O14)</f>
-        <v>0</v>
-      </c>
-      <c r="P15">
-        <f>SUM(P4:P14)</f>
-        <v>0</v>
-      </c>
-      <c r="Q15">
-        <f>SUM(Q4:Q14)</f>
-        <v>0</v>
-      </c>
-      <c r="R15">
-        <f>SUM(R1:R11)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>12</v>
-      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="cellIs" dxfId="47" priority="129" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="containsText" dxfId="46" priority="126" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",C20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="45" priority="127" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",C20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="44" priority="128" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",C20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20">
+    <cfRule type="cellIs" dxfId="43" priority="125" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18">
+    <cfRule type="containsText" dxfId="42" priority="122" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",C18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="41" priority="123" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",C18)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="40" priority="124" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",C18)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18">
+    <cfRule type="cellIs" dxfId="39" priority="121" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="containsText" dxfId="38" priority="130" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",C19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="37" priority="131" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",C19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="36" priority="132" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",C19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="containsText" dxfId="35" priority="18" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",C8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="34" priority="19" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",C8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="33" priority="20" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",C8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="cellIs" dxfId="32" priority="17" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11">
+    <cfRule type="containsText" dxfId="31" priority="14" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",C11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="15" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",C11)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="29" priority="16" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",C11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11">
+    <cfRule type="cellIs" dxfId="25" priority="13" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12">
+    <cfRule type="containsText" dxfId="23" priority="10" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",C12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="11" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",C12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="12" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",C12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12">
+    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="cellIs" dxfId="51" priority="113" operator="equal">
+    <cfRule type="containsText" dxfId="15" priority="6" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",C13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="7" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",C13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="To Do">
+      <formula>NOT(ISERROR(SEARCH("To Do",C13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="containsText" dxfId="50" priority="110" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",C14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="111" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",C14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="112" operator="containsText" text="To Do">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="To Do">
       <formula>NOT(ISERROR(SEARCH("To Do",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="47" priority="109" operator="equal">
-      <formula>"Done"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C12">
-    <cfRule type="containsText" dxfId="46" priority="106" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",C12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="107" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",C12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="108" operator="containsText" text="To Do">
-      <formula>NOT(ISERROR(SEARCH("To Do",C12)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C12">
-    <cfRule type="cellIs" dxfId="43" priority="105" operator="equal">
-      <formula>"Done"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C13">
-    <cfRule type="containsText" dxfId="42" priority="114" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",C13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="115" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",C13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="116" operator="containsText" text="To Do">
-      <formula>NOT(ISERROR(SEARCH("To Do",C13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",C8)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",C8)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="To Do">
-      <formula>NOT(ISERROR(SEARCH("To Do",C8)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1478,7 +1694,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V3">
       <formula1>To_Do</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12:C14 C8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18:C20 C8 C11:C14">
       <formula1>Todos</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>